<commit_message>
Validated Q21 and updated benchmark results
</commit_message>
<xml_diff>
--- a/scripts/SDQL-calculations.xlsx
+++ b/scripts/SDQL-calculations.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/repos/sdql/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A742344-4359-C74A-AA28-F12E2C0B2F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E3D562-960D-F440-9BBD-66976E0F1B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="2020" windowWidth="33340" windowHeight="21560" xr2:uid="{736C96A2-59EF-2F41-9F72-8B34CD25F15C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>q1</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>mean</t>
+  </si>
+  <si>
+    <t>q21</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304FF334-0C6A-3A48-8DC6-6C03B7BA7EC9}">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -493,7 +496,7 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,10 +558,13 @@
         <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>42</v>
       </c>
@@ -620,10 +626,13 @@
         <v>20</v>
       </c>
       <c r="V2">
+        <v>285</v>
+      </c>
+      <c r="X2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>41</v>
       </c>
@@ -685,10 +694,13 @@
         <v>19</v>
       </c>
       <c r="V3">
+        <v>286</v>
+      </c>
+      <c r="W3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>41</v>
       </c>
@@ -750,10 +762,13 @@
         <v>19</v>
       </c>
       <c r="V4">
+        <v>286</v>
+      </c>
+      <c r="W4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>42</v>
       </c>
@@ -815,10 +830,13 @@
         <v>19</v>
       </c>
       <c r="V5">
+        <v>285</v>
+      </c>
+      <c r="W5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>41</v>
       </c>
@@ -880,10 +898,13 @@
         <v>19</v>
       </c>
       <c r="V6">
+        <v>286</v>
+      </c>
+      <c r="W6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -892,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:V7" si="0">ROUND(_xlfn.STDEV.P(C$2:C$6), 0)</f>
+        <f t="shared" ref="C7:W7" si="0">ROUND(_xlfn.STDEV.P(C$2:C$6), 0)</f>
         <v>0</v>
       </c>
       <c r="D7">
@@ -971,8 +992,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="W7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -981,7 +1006,7 @@
         <v>41</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:V8" si="1">ROUND(AVERAGE(C$2:C$6), 0)</f>
+        <f t="shared" ref="C8:W8" si="1">ROUND(AVERAGE(C$2:C$6), 0)</f>
         <v>8</v>
       </c>
       <c r="D8">
@@ -1057,6 +1082,10 @@
         <v>19</v>
       </c>
       <c r="V8">
+        <f t="shared" si="1"/>
+        <v>286</v>
+      </c>
+      <c r="W8">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>

</xml_diff>